<commit_message>
[feat] create_detectors now supports e2detectors
What: intersection parameter xlsx file supports detector length

Why: want to have area detectors

Signed-off-by: Max Schrader <mcschrader@crimson.ua.edu>
</commit_message>
<xml_diff>
--- a/intersection_parameters/intersection_setup_file.xlsx
+++ b/intersection_parameters/intersection_setup_file.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -409,47 +409,67 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>Detector_Length</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>Sumo_Detector_2</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>RW_Detector_2</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Detector_2_Distance</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Detector_2_Length</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Detect_Actual_Lane</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Detect_2_Actual_Lane</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Detect_Actual_Edge</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Detect_2_Actual_Edge</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Detect_Actual_Distance</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Detect_2_Actual_Distance</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Detect_Length</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Detect_2_Length</t>
         </is>
       </c>
     </row>
@@ -488,29 +508,35 @@
         <v>8</v>
       </c>
       <c r="H2" t="n">
-        <v>30</v>
-      </c>
-      <c r="I2" t="inlineStr"/>
+        <v>100</v>
+      </c>
+      <c r="I2" t="n">
+        <v>10</v>
+      </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Bryce_NB_0</t>
-        </is>
-      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Bryce_NB</t>
+          <t>Bryce_NB_0</t>
         </is>
       </c>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr">
         <is>
-          <t>-9.1</t>
+          <t>Bryce_NB</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="n">
+        <v>-30.5</v>
+      </c>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="n">
+        <v>10</v>
+      </c>
+      <c r="U2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -547,29 +573,35 @@
         <v>8</v>
       </c>
       <c r="H3" t="n">
-        <v>30</v>
-      </c>
-      <c r="I3" t="inlineStr"/>
+        <v>100</v>
+      </c>
+      <c r="I3" t="n">
+        <v>10</v>
+      </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>Bryce_NB_1</t>
-        </is>
-      </c>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr">
         <is>
-          <t>Bryce_NB</t>
+          <t>Bryce_NB_1</t>
         </is>
       </c>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr">
         <is>
-          <t>-9.1</t>
+          <t>Bryce_NB</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="n">
+        <v>-30.5</v>
+      </c>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="n">
+        <v>10</v>
+      </c>
+      <c r="U3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -608,27 +640,33 @@
       <c r="H4" t="n">
         <v>30</v>
       </c>
-      <c r="I4" t="inlineStr"/>
+      <c r="I4" t="n">
+        <v>30</v>
+      </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Bryce_NB_2</t>
-        </is>
-      </c>
+      <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr">
         <is>
-          <t>Bryce_NB</t>
+          <t>Bryce_NB_2</t>
         </is>
       </c>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr">
         <is>
-          <t>-9.1</t>
+          <t>Bryce_NB</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="n">
+        <v>-9.1</v>
+      </c>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="n">
+        <v>30</v>
+      </c>
+      <c r="U4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -665,29 +703,35 @@
         <v>2</v>
       </c>
       <c r="H5" t="n">
-        <v>30</v>
-      </c>
-      <c r="I5" t="inlineStr"/>
+        <v>100</v>
+      </c>
+      <c r="I5" t="n">
+        <v>10</v>
+      </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Campus_EB_0</t>
-        </is>
-      </c>
+      <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr">
         <is>
-          <t>Campus_EB</t>
+          <t>Campus_EB_0</t>
         </is>
       </c>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr">
         <is>
-          <t>-9.1</t>
+          <t>Campus_EB</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="n">
+        <v>-30.5</v>
+      </c>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="n">
+        <v>10</v>
+      </c>
+      <c r="U5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -726,27 +770,33 @@
       <c r="H6" t="n">
         <v>30</v>
       </c>
-      <c r="I6" t="inlineStr"/>
+      <c r="I6" t="n">
+        <v>30</v>
+      </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>Campus_EB_1</t>
-        </is>
-      </c>
+      <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Campus_EB</t>
+          <t>Campus_EB_1</t>
         </is>
       </c>
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr">
         <is>
-          <t>-9.1</t>
+          <t>Campus_EB</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="n">
+        <v>-9.1</v>
+      </c>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="n">
+        <v>30</v>
+      </c>
+      <c r="U6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -783,29 +833,35 @@
         <v>4</v>
       </c>
       <c r="H7" t="n">
-        <v>30</v>
-      </c>
-      <c r="I7" t="inlineStr"/>
+        <v>100</v>
+      </c>
+      <c r="I7" t="n">
+        <v>10</v>
+      </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>Bryce_SB_0</t>
-        </is>
-      </c>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr">
         <is>
-          <t>Bryce_SB</t>
+          <t>Bryce_SB_0</t>
         </is>
       </c>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr">
         <is>
-          <t>-9.1</t>
+          <t>Bryce_SB</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="n">
+        <v>-30.5</v>
+      </c>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="n">
+        <v>10</v>
+      </c>
+      <c r="U7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -842,29 +898,35 @@
         <v>4</v>
       </c>
       <c r="H8" t="n">
-        <v>30</v>
-      </c>
-      <c r="I8" t="inlineStr"/>
+        <v>100</v>
+      </c>
+      <c r="I8" t="n">
+        <v>10</v>
+      </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>Bryce_SB_1</t>
-        </is>
-      </c>
+      <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr">
         <is>
-          <t>Bryce_SB</t>
+          <t>Bryce_SB_1</t>
         </is>
       </c>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr">
         <is>
-          <t>-9.1</t>
+          <t>Bryce_SB</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="n">
+        <v>-30.5</v>
+      </c>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="n">
+        <v>10</v>
+      </c>
+      <c r="U8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -903,27 +965,33 @@
       <c r="H9" t="n">
         <v>30</v>
       </c>
-      <c r="I9" t="inlineStr"/>
+      <c r="I9" t="n">
+        <v>30</v>
+      </c>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>Bryce_SB_2</t>
-        </is>
-      </c>
+      <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr">
         <is>
-          <t>Bryce_SB</t>
+          <t>Bryce_SB_2</t>
         </is>
       </c>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr">
         <is>
-          <t>-9.1</t>
+          <t>Bryce_SB</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="n">
+        <v>-9.1</v>
+      </c>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="n">
+        <v>30</v>
+      </c>
+      <c r="U9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -957,28 +1025,32 @@
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr">
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
         <is>
           <t>Campus_WB_0</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>Campus_WB_0</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
+      <c r="P10" t="inlineStr">
         <is>
           <t>Campus_WB</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="Q10" t="inlineStr">
         <is>
           <t>Campus_WB</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1015,29 +1087,35 @@
         <v>6</v>
       </c>
       <c r="H11" t="n">
-        <v>30</v>
-      </c>
-      <c r="I11" t="inlineStr"/>
+        <v>100</v>
+      </c>
+      <c r="I11" t="n">
+        <v>10</v>
+      </c>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>Campus_WB_1</t>
-        </is>
-      </c>
+      <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr">
         <is>
-          <t>Campus_WB</t>
+          <t>gneE1.93_1</t>
         </is>
       </c>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr">
         <is>
-          <t>-9.1</t>
+          <t>gneE1.93</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="n">
+        <v>-9.259999024640031</v>
+      </c>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="n">
+        <v>10</v>
+      </c>
+      <c r="U11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1076,27 +1154,33 @@
       <c r="H12" t="n">
         <v>30</v>
       </c>
-      <c r="I12" t="inlineStr"/>
+      <c r="I12" t="n">
+        <v>30</v>
+      </c>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>Campus_WB_2</t>
-        </is>
-      </c>
+      <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr">
         <is>
-          <t>Campus_WB</t>
+          <t>Campus_WB_2</t>
         </is>
       </c>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr">
         <is>
-          <t>-9.1</t>
+          <t>Campus_WB</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="n">
+        <v>-9.1</v>
+      </c>
+      <c r="S12" t="inlineStr"/>
+      <c r="T12" t="n">
+        <v>30</v>
+      </c>
+      <c r="U12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
[feat] create_detector.py now considers junction length for e2 detectors
what: Before, the detector create algorithm did not consider the length of the junctions themselves when placing detectors.

With this commit it does and will throw a message when the detector should be placed on the junction.

Signed-off-by: Max Schrader <mcschrader@crimson.ua.edu>
</commit_message>
<xml_diff>
--- a/intersection_parameters/intersection_setup_file.xlsx
+++ b/intersection_parameters/intersection_setup_file.xlsx
@@ -530,7 +530,7 @@
       </c>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="n">
-        <v>-30.5</v>
+        <v>1.77390151467452</v>
       </c>
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="n">
@@ -595,7 +595,7 @@
       </c>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="n">
-        <v>-30.5</v>
+        <v>1.733144255704353</v>
       </c>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="n">
@@ -660,7 +660,7 @@
       </c>
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="n">
-        <v>-0</v>
+        <v>39.27</v>
       </c>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="n">
@@ -725,7 +725,7 @@
       </c>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="n">
-        <v>-30.5</v>
+        <v>3.953271223769448</v>
       </c>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="n">
@@ -790,7 +790,7 @@
       </c>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="n">
-        <v>-0</v>
+        <v>34.44</v>
       </c>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="n">
@@ -855,7 +855,7 @@
       </c>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="n">
-        <v>-30.5</v>
+        <v>41.46613151759277</v>
       </c>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="n">
@@ -920,7 +920,7 @@
       </c>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="n">
-        <v>-30.5</v>
+        <v>41.43457877430134</v>
       </c>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="n">
@@ -985,7 +985,7 @@
       </c>
       <c r="Q9" t="inlineStr"/>
       <c r="R9" t="n">
-        <v>-0</v>
+        <v>71.92</v>
       </c>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="n">
@@ -1109,7 +1109,7 @@
       </c>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="n">
-        <v>-9.259999024640031</v>
+        <v>11.61185150262494</v>
       </c>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="n">
@@ -1174,7 +1174,7 @@
       </c>
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="n">
-        <v>-0</v>
+        <v>21.22</v>
       </c>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="n">

</xml_diff>

<commit_message>
[fix] create_detector handles lanes with more complex geometry
What: I didn't understand how sumolib.net.edge.lane.getShape worked. returns all the geometry points. Have to interate through all to get the length.

Its fixed.

Why: I reiterate. Max is dum dum

Signed-off-by: Max Schrader <mcschrader@crimson.ua.edu>
</commit_message>
<xml_diff>
--- a/intersection_parameters/intersection_setup_file.xlsx
+++ b/intersection_parameters/intersection_setup_file.xlsx
@@ -530,7 +530,7 @@
       </c>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="n">
-        <v>1.77390151467452</v>
+        <v>21.62267899129298</v>
       </c>
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="n">
@@ -595,7 +595,7 @@
       </c>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="n">
-        <v>1.733144255704353</v>
+        <v>19.69708450735381</v>
       </c>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="n">
@@ -725,7 +725,7 @@
       </c>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="n">
-        <v>3.953271223769448</v>
+        <v>22.94250238250783</v>
       </c>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="n">
@@ -855,7 +855,7 @@
       </c>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="n">
-        <v>41.46613151759277</v>
+        <v>56.05221049722274</v>
       </c>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="n">
@@ -920,7 +920,7 @@
       </c>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="n">
-        <v>41.43457877430134</v>
+        <v>54.54562755004776</v>
       </c>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="n">
@@ -1098,18 +1098,18 @@
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr">
         <is>
-          <t>gneE1.93_1</t>
+          <t>Campus_WB_1</t>
         </is>
       </c>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr">
         <is>
-          <t>gneE1.93</t>
+          <t>Campus_WB</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="n">
-        <v>11.61185150262494</v>
+        <v>13.28494941060483</v>
       </c>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="n">

</xml_diff>

<commit_message>
[fix] updated the create_detector script again... + others
What: From working on US69, made a couel more tweaks to the create_detector script. It is nasty but works

Also removed the check to transmit only when current status != last status. That logic got stuck somewhere.

Why: Max has jumped the gun on committing. He will refer to himself in third person when he a dumb dumb.

Signed-off-by: Max Schrader <mcschrader@crimson.ua.edu>
</commit_message>
<xml_diff>
--- a/intersection_parameters/intersection_setup_file.xlsx
+++ b/intersection_parameters/intersection_setup_file.xlsx
@@ -508,7 +508,7 @@
         <v>8</v>
       </c>
       <c r="H2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
         <v>10</v>
@@ -530,7 +530,7 @@
       </c>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="n">
-        <v>21.62267899129298</v>
+        <v>39.27</v>
       </c>
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="n">
@@ -573,7 +573,7 @@
         <v>8</v>
       </c>
       <c r="H3" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
         <v>10</v>
@@ -595,7 +595,7 @@
       </c>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="n">
-        <v>19.69708450735381</v>
+        <v>39.27</v>
       </c>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="n">
@@ -703,7 +703,7 @@
         <v>2</v>
       </c>
       <c r="H5" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="I5" t="n">
         <v>10</v>
@@ -714,18 +714,18 @@
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr">
         <is>
-          <t>Campus_EB_0</t>
+          <t>gneE2_0</t>
         </is>
       </c>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Campus_EB</t>
+          <t>gneE2</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="n">
-        <v>22.94250238250783</v>
+        <v>152.8368118543222</v>
       </c>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="n">
@@ -833,7 +833,7 @@
         <v>4</v>
       </c>
       <c r="H7" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
         <v>10</v>
@@ -855,7 +855,7 @@
       </c>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="n">
-        <v>56.05221049722274</v>
+        <v>71.92</v>
       </c>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="n">
@@ -898,7 +898,7 @@
         <v>4</v>
       </c>
       <c r="H8" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
         <v>10</v>
@@ -920,7 +920,7 @@
       </c>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="n">
-        <v>54.54562755004776</v>
+        <v>71.92</v>
       </c>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="n">
@@ -1087,7 +1087,7 @@
         <v>6</v>
       </c>
       <c r="H11" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="I11" t="n">
         <v>10</v>
@@ -1098,18 +1098,18 @@
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr">
         <is>
-          <t>Campus_WB_1</t>
+          <t>gneE1.93_1</t>
         </is>
       </c>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Campus_WB</t>
+          <t>gneE1.93</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="n">
-        <v>13.28494941060483</v>
+        <v>11.98563409193079</v>
       </c>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="n">

</xml_diff>